<commit_message>
Two more routes pending
</commit_message>
<xml_diff>
--- a/backend/uploads/students.xlsx
+++ b/backend/uploads/students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\management_portal\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D05184-52CE-4B4C-8996-F19FE2C87535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3F0C0E-343A-44D1-9EA1-245B21D16D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8AD0A362-A03C-4CB8-A18D-FDDE53864B6E}"/>
   </bookViews>
@@ -69,10 +69,10 @@
     <t>B</t>
   </si>
   <si>
-    <t>vdwvw</t>
-  </si>
-  <si>
-    <t>gtnhtrnjy</t>
+    <t>wahid</t>
+  </si>
+  <si>
+    <t>abass</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,10 +501,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="1">
-        <v>7387</v>
+        <v>9442571997</v>
       </c>
       <c r="C2" s="1">
-        <v>355</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -525,7 +525,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="5">
-        <v>25757</v>
+        <v>5632562356</v>
       </c>
       <c r="C3" s="1">
         <v>25</v>

</xml_diff>